<commit_message>
corro limpieza y cálculo sep-2022
</commit_message>
<xml_diff>
--- a/MenstruAccion/cuanto_cuesta_menstruar/2022 Septiembre/Fuentes/serie_inflacion.xlsx
+++ b/MenstruAccion/cuanto_cuesta_menstruar/2022 Septiembre/Fuentes/serie_inflacion.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\espin\OneDrive\Documents\Lu\Ecofeminita\EcoFemiData\EcoFemiData\EcoFemiData\MenstruAccion\cuanto_cuesta_menstruar\2022 Marzo\Fuentes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\espin\OneDrive\Documents\Lu\Ecofeminita\EcoFemiData\EcoFemiData\EcoFemiData\MenstruAccion\cuanto_cuesta_menstruar\2022 Septiembre\Fuentes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A244C4BF-3F63-4A81-BB12-9EB723BE63DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FCA32E4-2E4C-4DFE-A821-87F3570C81CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -141,21 +154,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
@@ -544,555 +552,640 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>43525</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>205.9571</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>210.62799999999999</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>210.369</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>43556</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>213.05170000000001</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>215.99850000000001</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>217.7389</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>43586</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>219.56909999999999</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>221.25880000000001</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>228.7921</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>43617</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>225.53700000000001</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>226.9033</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>236.91650000000001</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>43647</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>230.494</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>232.02950000000001</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>246.6508</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>43678</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>239.60769999999999</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>242.5051</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>259.46030000000002</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>43709</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>253.71019999999999</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>256.37569999999999</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>281.09820000000002</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>43739</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>262.06610000000001</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>262.66030000000001</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>294.2595</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>43770</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>273.2158</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>276.63389999999998</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>312.84699999999998</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>43800</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>283.44420000000002</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>285.29700000000003</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>330.32400000000001</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>43831</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>289.82990000000001</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>298.65010000000001</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>323.7294</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>43862</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>295.666</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>306.6182</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <v>325.1671</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>43891</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>305.55149999999998</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>318.67770000000002</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="3">
         <v>333.81630000000001</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>43922</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>310.12430000000001</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>328.77850000000001</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <v>337.75229999999999</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <v>43952</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>314.90870000000001</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <v>331.01459999999997</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3">
         <v>341.34609999999998</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <v>43983</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>321.97379999999998</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <v>334.46359999999999</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <v>348.97590000000002</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
+      <c r="A18" s="1">
         <v>44013</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>328.20139999999998</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <v>338.76479999999998</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="3">
         <v>356.54669999999999</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
+      <c r="A19" s="1">
         <v>44044</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="2">
         <v>337.06319999999999</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="3">
         <v>350.50760000000002</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="3">
         <v>365.11130000000003</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <v>44075</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="2">
         <v>346.6207</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="3">
         <v>360.86919999999998</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="3">
         <v>377.85090000000002</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <v>44105</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="2">
         <v>359.65699999999998</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="3">
         <v>378.08960000000002</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="3">
         <v>389.51089999999999</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <v>44136</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <v>371.02109999999999</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="3">
         <v>388.38639999999998</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="3">
         <v>403.80290000000002</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
+      <c r="A23" s="1">
         <v>44166</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="2">
         <v>385.88260000000002</v>
       </c>
-      <c r="C23" s="4">
+      <c r="C23" s="3">
         <v>405.28710000000001</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="3">
         <v>424.96679999999998</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
+      <c r="A24" s="1">
         <v>44197</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="2">
         <v>401.50709999999998</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="3">
         <v>424.8374</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="3">
         <v>439.37759999999997</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
+      <c r="A25" s="1">
         <v>44228</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="2">
         <v>415.85950000000003</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="3">
         <v>441.07220000000001</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="3">
         <v>454.72649999999999</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
+      <c r="A26" s="1">
         <v>44256</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="2">
         <v>435.8657</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="3">
         <v>461.32380000000001</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="3">
         <v>472.85599999999999</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
+      <c r="A27" s="1">
         <v>44287</v>
       </c>
-      <c r="B27" s="8">
+      <c r="B27" s="4">
         <v>453.65030000000002</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C27" s="5">
         <v>481.2407</v>
       </c>
-      <c r="D27" s="9">
+      <c r="D27" s="5">
         <v>490.48200000000003</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
+      <c r="A28" s="1">
         <v>44317</v>
       </c>
-      <c r="B28" s="8">
+      <c r="B28" s="4">
         <v>468.72500000000002</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="5">
         <v>496.17959999999999</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D28" s="5">
         <v>513.79179999999997</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
+      <c r="A29" s="1">
         <v>44348</v>
       </c>
-      <c r="B29" s="8">
+      <c r="B29" s="4">
         <v>483.60489999999999</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29" s="5">
         <v>512.25930000000005</v>
       </c>
-      <c r="D29" s="9">
+      <c r="D29" s="5">
         <v>530.27660000000003</v>
       </c>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
-      <c r="L29" s="11"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
+      <c r="A30" s="1">
         <v>44378</v>
       </c>
-      <c r="B30" s="8">
+      <c r="B30" s="4">
         <v>498.09870000000001</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="5">
         <v>529.70870000000002</v>
       </c>
-      <c r="D30" s="9">
+      <c r="D30" s="5">
         <v>550.54639999999995</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="2">
+      <c r="A31" s="1">
         <v>44409</v>
       </c>
-      <c r="B31" s="8">
+      <c r="B31" s="4">
         <v>510.39420000000001</v>
       </c>
-      <c r="C31" s="9">
+      <c r="C31" s="5">
         <v>537.58669999999995</v>
       </c>
-      <c r="D31" s="9">
+      <c r="D31" s="5">
         <v>573.65009999999995</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="2">
+      <c r="A32" s="1">
         <v>44440</v>
       </c>
-      <c r="B32" s="8">
+      <c r="B32" s="4">
         <v>528.49680000000001</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C32" s="5">
         <v>553.43730000000005</v>
       </c>
-      <c r="D32" s="9">
+      <c r="D32" s="5">
         <v>598.35550000000001</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="2">
+      <c r="A33" s="1">
         <v>44470</v>
       </c>
-      <c r="B33" s="10">
+      <c r="B33" s="6">
         <v>547.08019999999999</v>
       </c>
-      <c r="C33" s="11">
+      <c r="C33" s="7">
         <v>572.32929999999999</v>
       </c>
-      <c r="D33" s="12">
+      <c r="D33" s="7">
         <v>626.67489999999998</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" s="2">
+      <c r="A34" s="1">
         <v>44501</v>
       </c>
-      <c r="B34" s="10">
+      <c r="B34" s="6">
         <v>560.91840000000002</v>
       </c>
-      <c r="C34" s="11">
+      <c r="C34" s="7">
         <v>584.47170000000006</v>
       </c>
-      <c r="D34" s="12">
+      <c r="D34" s="7">
         <v>641.93740000000003</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="2">
+      <c r="A35" s="1">
         <v>44531</v>
       </c>
-      <c r="B35" s="10">
+      <c r="B35" s="6">
         <v>582.45749999999998</v>
       </c>
-      <c r="C35" s="11">
+      <c r="C35" s="7">
         <v>609.33109999999999</v>
       </c>
-      <c r="D35" s="12">
+      <c r="D35" s="7">
         <v>645.14340000000004</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="2">
+      <c r="A36" s="1">
         <v>44562</v>
       </c>
-      <c r="B36" s="10">
+      <c r="B36" s="6">
         <v>605.0317</v>
       </c>
-      <c r="C36" s="11">
+      <c r="C36" s="7">
         <v>639.40499999999997</v>
       </c>
-      <c r="D36" s="12">
+      <c r="D36" s="7">
         <v>671.67290000000003</v>
       </c>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="12"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A37" s="2">
+      <c r="A37" s="1">
         <v>44593</v>
       </c>
-      <c r="B37" s="10">
+      <c r="B37" s="6">
         <v>633.43409999999994</v>
       </c>
-      <c r="C37" s="11">
+      <c r="C37" s="7">
         <v>687.16579999999999</v>
       </c>
-      <c r="D37" s="12">
+      <c r="D37" s="7">
         <v>696.11609999999996</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A38" s="2">
+      <c r="A38" s="1">
         <v>44621</v>
       </c>
+      <c r="B38" s="6">
+        <v>676.0566</v>
+      </c>
+      <c r="C38" s="7">
+        <v>736.94510000000002</v>
+      </c>
+      <c r="D38" s="7">
+        <v>730.59220000000005</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>44652</v>
+      </c>
+      <c r="B39" s="6">
+        <v>716.93989999999997</v>
+      </c>
+      <c r="C39" s="7">
+        <v>780.14570000000003</v>
+      </c>
+      <c r="D39" s="7">
+        <v>777.29909999999995</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>44682</v>
+      </c>
+      <c r="B40" s="6">
+        <v>753.14700000000005</v>
+      </c>
+      <c r="C40" s="7">
+        <v>814.5693</v>
+      </c>
+      <c r="D40" s="7">
+        <v>825.57389999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>44713</v>
+      </c>
+      <c r="B41" s="6">
+        <v>793.02779999999996</v>
+      </c>
+      <c r="C41" s="7">
+        <v>852.18039999999996</v>
+      </c>
+      <c r="D41" s="7">
+        <v>886.798</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>44743</v>
+      </c>
+      <c r="B42" s="6">
+        <v>851.76099999999997</v>
+      </c>
+      <c r="C42" s="7">
+        <v>903.46090000000004</v>
+      </c>
+      <c r="D42" s="7">
+        <v>947.49300000000005</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>44774</v>
+      </c>
+      <c r="B43" s="6">
+        <v>911.13160000000005</v>
+      </c>
+      <c r="C43" s="7">
+        <v>967.58050000000003</v>
+      </c>
+      <c r="D43" s="7">
+        <v>1001.7380000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>44805</v>
+      </c>
+      <c r="B44" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>